<commit_message>
Polish Brand Bulk Upload
</commit_message>
<xml_diff>
--- a/public/download/brand_bulk_demo.xlsx
+++ b/public/download/brand_bulk_demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laravel\e-commerce\public\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laravel\cpl-commerce-singapore\public\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D00080-80EF-472B-B069-0791F229ED5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04CF48A-50DB-4C56-A28D-BF3ECD7E7502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -39,24 +39,15 @@
     <t>meta_description</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>meta_keyword</t>
   </si>
   <si>
     <t>status</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>featured</t>
   </si>
   <si>
-    <t>Inactive</t>
-  </si>
-  <si>
     <t>A4Tech</t>
   </si>
   <si>
@@ -70,9 +61,6 @@
   </si>
   <si>
     <t>A4Tech Shop Bangladesh</t>
-  </si>
-  <si>
-    <t>Brand Description</t>
   </si>
   <si>
     <t>components</t>
@@ -401,24 +389,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,57 +413,51 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>